<commit_message>
Final commit i guess
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aitor\Documents\GitHub\cameraCalibrate\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2140F4A7-1480-49A6-BA90-F3F7F9694494}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55A400C3-5CCA-4788-AE6C-63169DEAF9AF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1905" yWindow="1905" windowWidth="10095" windowHeight="7095" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Comparison" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="26">
   <si>
     <t>BrownConrady:</t>
   </si>
@@ -110,6 +110,9 @@
   </si>
   <si>
     <t>This is from one of the tests</t>
+  </si>
+  <si>
+    <t>SCARAMUZZA</t>
   </si>
 </sst>
 </file>
@@ -662,10 +665,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EDA579C3-D662-4E03-AD80-8788C3CACEA4}">
-  <dimension ref="C3:Q16"/>
+  <dimension ref="C3:Q30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J7" sqref="J7"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="P22" sqref="P22:P30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -784,15 +787,15 @@
         <v>1318.376</v>
       </c>
       <c r="H8" s="1">
-        <f t="shared" ref="H8:H16" si="0">ABS(D8-1500)/1500</f>
+        <f t="shared" ref="H8:H15" si="0">ABS(D8-1500)/1500</f>
         <v>2.7314666666666654E-2</v>
       </c>
       <c r="I8" s="1">
-        <f t="shared" ref="I8:I16" si="1">ABS(E8-1125)/1125</f>
+        <f t="shared" ref="I8:I15" si="1">ABS(E8-1125)/1125</f>
         <v>1.1684444444444428E-2</v>
       </c>
       <c r="J8" s="1">
-        <f t="shared" ref="J8:J16" si="2">F8/G8</f>
+        <f t="shared" ref="J8:J15" si="2">F8/G8</f>
         <v>1.0173068987906333</v>
       </c>
       <c r="M8">
@@ -1123,6 +1126,420 @@
       <c r="H16" s="1"/>
       <c r="I16" s="1"/>
       <c r="J16" s="1"/>
+    </row>
+    <row r="18" spans="3:17" x14ac:dyDescent="0.25">
+      <c r="C18" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="21" spans="3:17" x14ac:dyDescent="0.25">
+      <c r="C21" t="s">
+        <v>19</v>
+      </c>
+      <c r="D21" t="s">
+        <v>3</v>
+      </c>
+      <c r="E21" t="s">
+        <v>4</v>
+      </c>
+      <c r="F21" t="s">
+        <v>1</v>
+      </c>
+      <c r="G21" t="s">
+        <v>2</v>
+      </c>
+      <c r="H21" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="I21" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="J21" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="M21" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="N21" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="O21" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="P21" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="Q21" s="1"/>
+    </row>
+    <row r="22" spans="3:17" x14ac:dyDescent="0.25">
+      <c r="C22">
+        <v>3</v>
+      </c>
+      <c r="D22">
+        <v>1478.8720000000001</v>
+      </c>
+      <c r="E22">
+        <v>1843.9839999999999</v>
+      </c>
+      <c r="F22">
+        <v>1280.0119999999999</v>
+      </c>
+      <c r="G22">
+        <v>1293.22</v>
+      </c>
+      <c r="H22" s="1">
+        <f>ABS(D22-1500)/1500</f>
+        <v>1.4085333333333287E-2</v>
+      </c>
+      <c r="I22" s="1">
+        <f>ABS(E22-1125)/1125</f>
+        <v>0.63909688888888883</v>
+      </c>
+      <c r="J22" s="1">
+        <f>F22/G22</f>
+        <v>0.98978673388905203</v>
+      </c>
+      <c r="M22">
+        <v>9.7799999999999998E-2</v>
+      </c>
+      <c r="N22">
+        <v>-0.1164</v>
+      </c>
+      <c r="O22">
+        <v>4.7000000000000002E-3</v>
+      </c>
+      <c r="P22">
+        <v>6.9500000000000006E-2</v>
+      </c>
+    </row>
+    <row r="23" spans="3:17" x14ac:dyDescent="0.25">
+      <c r="C23">
+        <v>4</v>
+      </c>
+      <c r="D23">
+        <v>1494.4839999999999</v>
+      </c>
+      <c r="E23">
+        <v>1220.1079999999999</v>
+      </c>
+      <c r="F23">
+        <v>1270.6279999999999</v>
+      </c>
+      <c r="G23">
+        <v>1282.8810000000001</v>
+      </c>
+      <c r="H23" s="1">
+        <f t="shared" ref="H23:H30" si="3">ABS(D23-1500)/1500</f>
+        <v>3.6773333333333844E-3</v>
+      </c>
+      <c r="I23" s="1">
+        <f t="shared" ref="I23:I30" si="4">ABS(E23-1125)/1125</f>
+        <v>8.4540444444444404E-2</v>
+      </c>
+      <c r="J23" s="1">
+        <f t="shared" ref="J23:J30" si="5">F23/G23</f>
+        <v>0.99044884131887512</v>
+      </c>
+      <c r="M23">
+        <v>0.10639999999999999</v>
+      </c>
+      <c r="N23">
+        <v>-0.1489</v>
+      </c>
+      <c r="O23">
+        <v>7.6499999999999999E-2</v>
+      </c>
+      <c r="P23">
+        <v>2.01E-2</v>
+      </c>
+    </row>
+    <row r="24" spans="3:17" x14ac:dyDescent="0.25">
+      <c r="C24">
+        <v>5</v>
+      </c>
+      <c r="D24">
+        <v>1500.19</v>
+      </c>
+      <c r="E24">
+        <v>1215.3810000000001</v>
+      </c>
+      <c r="F24">
+        <v>1273.0609999999999</v>
+      </c>
+      <c r="G24">
+        <v>1287.6610000000001</v>
+      </c>
+      <c r="H24" s="1">
+        <f t="shared" si="3"/>
+        <v>1.2666666666670304E-4</v>
+      </c>
+      <c r="I24" s="1">
+        <f t="shared" si="4"/>
+        <v>8.0338666666666739E-2</v>
+      </c>
+      <c r="J24" s="1">
+        <f t="shared" si="5"/>
+        <v>0.98866161202366143</v>
+      </c>
+      <c r="M24">
+        <v>0.1028</v>
+      </c>
+      <c r="N24">
+        <v>-0.18679999999999999</v>
+      </c>
+      <c r="O24">
+        <v>0.1759</v>
+      </c>
+      <c r="P24">
+        <v>-4.7399999999999998E-2</v>
+      </c>
+    </row>
+    <row r="25" spans="3:17" x14ac:dyDescent="0.25">
+      <c r="C25">
+        <v>6</v>
+      </c>
+      <c r="D25">
+        <v>1500.4079999999999</v>
+      </c>
+      <c r="E25">
+        <v>1210.4059999999999</v>
+      </c>
+      <c r="F25">
+        <v>1274.1559999999999</v>
+      </c>
+      <c r="G25">
+        <v>1287.038</v>
+      </c>
+      <c r="H25" s="1">
+        <f t="shared" si="3"/>
+        <v>2.7199999999993451E-4</v>
+      </c>
+      <c r="I25" s="1">
+        <f t="shared" si="4"/>
+        <v>7.5916444444444398E-2</v>
+      </c>
+      <c r="J25" s="1">
+        <f t="shared" si="5"/>
+        <v>0.98999097151754645</v>
+      </c>
+      <c r="M25">
+        <v>0.12139999999999999</v>
+      </c>
+      <c r="N25">
+        <v>-0.28610000000000002</v>
+      </c>
+      <c r="O25">
+        <v>0.34870000000000001</v>
+      </c>
+      <c r="P25">
+        <v>-0.1399</v>
+      </c>
+      <c r="Q25" s="3"/>
+    </row>
+    <row r="26" spans="3:17" x14ac:dyDescent="0.25">
+      <c r="C26">
+        <v>7</v>
+      </c>
+      <c r="D26">
+        <v>1497.4760000000001</v>
+      </c>
+      <c r="E26">
+        <v>1200.0830000000001</v>
+      </c>
+      <c r="F26">
+        <v>1285.921</v>
+      </c>
+      <c r="G26">
+        <v>1297.4190000000001</v>
+      </c>
+      <c r="H26" s="1">
+        <f t="shared" si="3"/>
+        <v>1.6826666666665915E-3</v>
+      </c>
+      <c r="I26" s="1">
+        <f t="shared" si="4"/>
+        <v>6.6740444444444519E-2</v>
+      </c>
+      <c r="J26" s="1">
+        <f t="shared" si="5"/>
+        <v>0.99113778971943522</v>
+      </c>
+      <c r="M26">
+        <v>8.0699999999999994E-2</v>
+      </c>
+      <c r="N26">
+        <v>-0.18909999999999999</v>
+      </c>
+      <c r="O26">
+        <v>0.25309999999999999</v>
+      </c>
+      <c r="P26">
+        <v>-0.1072</v>
+      </c>
+    </row>
+    <row r="27" spans="3:17" x14ac:dyDescent="0.25">
+      <c r="C27">
+        <v>8</v>
+      </c>
+      <c r="D27">
+        <v>1493.8779999999999</v>
+      </c>
+      <c r="E27">
+        <v>1190.828</v>
+      </c>
+      <c r="F27">
+        <v>1286.5219999999999</v>
+      </c>
+      <c r="G27">
+        <v>1296.252</v>
+      </c>
+      <c r="H27" s="1">
+        <f t="shared" si="3"/>
+        <v>4.0813333333333804E-3</v>
+      </c>
+      <c r="I27" s="1">
+        <f t="shared" si="4"/>
+        <v>5.8513777777777755E-2</v>
+      </c>
+      <c r="J27" s="1">
+        <f t="shared" si="5"/>
+        <v>0.99249374350049213</v>
+      </c>
+      <c r="M27">
+        <v>8.5599999999999996E-2</v>
+      </c>
+      <c r="N27">
+        <v>-0.19670000000000001</v>
+      </c>
+      <c r="O27">
+        <v>0.2702</v>
+      </c>
+      <c r="P27">
+        <v>-0.11840000000000001</v>
+      </c>
+    </row>
+    <row r="28" spans="3:17" x14ac:dyDescent="0.25">
+      <c r="C28">
+        <v>9</v>
+      </c>
+      <c r="D28">
+        <v>1506.5419999999999</v>
+      </c>
+      <c r="E28">
+        <v>1179.117</v>
+      </c>
+      <c r="F28">
+        <v>1294.086</v>
+      </c>
+      <c r="G28">
+        <v>1300.107</v>
+      </c>
+      <c r="H28" s="1">
+        <f t="shared" si="3"/>
+        <v>4.3613333333332779E-3</v>
+      </c>
+      <c r="I28" s="1">
+        <f t="shared" si="4"/>
+        <v>4.8103999999999966E-2</v>
+      </c>
+      <c r="J28" s="1">
+        <f t="shared" si="5"/>
+        <v>0.99536884271833015</v>
+      </c>
+      <c r="M28">
+        <v>5.1900000000000002E-2</v>
+      </c>
+      <c r="N28">
+        <v>-6.3799999999999996E-2</v>
+      </c>
+      <c r="O28">
+        <v>8.4099999999999994E-2</v>
+      </c>
+      <c r="P28">
+        <v>-3.4200000000000001E-2</v>
+      </c>
+    </row>
+    <row r="29" spans="3:17" x14ac:dyDescent="0.25">
+      <c r="C29">
+        <v>10</v>
+      </c>
+      <c r="D29">
+        <v>1507.433</v>
+      </c>
+      <c r="E29">
+        <v>1178.2239999999999</v>
+      </c>
+      <c r="F29">
+        <v>1294.7660000000001</v>
+      </c>
+      <c r="G29">
+        <v>1300.252</v>
+      </c>
+      <c r="H29" s="1">
+        <f t="shared" si="3"/>
+        <v>4.9553333333333281E-3</v>
+      </c>
+      <c r="I29" s="1">
+        <f t="shared" si="4"/>
+        <v>4.7310222222222163E-2</v>
+      </c>
+      <c r="J29" s="1">
+        <f t="shared" si="5"/>
+        <v>0.99578081787222794</v>
+      </c>
+      <c r="M29">
+        <v>4.2599999999999999E-2</v>
+      </c>
+      <c r="N29">
+        <v>-2.29E-2</v>
+      </c>
+      <c r="O29">
+        <v>3.1300000000000001E-2</v>
+      </c>
+      <c r="P29">
+        <v>-1.4500000000000001E-2</v>
+      </c>
+    </row>
+    <row r="30" spans="3:17" x14ac:dyDescent="0.25">
+      <c r="C30">
+        <v>11</v>
+      </c>
+      <c r="D30">
+        <v>1506.105</v>
+      </c>
+      <c r="E30">
+        <v>1173.2539999999999</v>
+      </c>
+      <c r="F30">
+        <v>1294.114</v>
+      </c>
+      <c r="G30">
+        <v>1298.127</v>
+      </c>
+      <c r="H30" s="1">
+        <f t="shared" si="3"/>
+        <v>4.070000000000012E-3</v>
+      </c>
+      <c r="I30" s="1">
+        <f t="shared" si="4"/>
+        <v>4.2892444444444358E-2</v>
+      </c>
+      <c r="J30" s="1">
+        <f t="shared" si="5"/>
+        <v>0.99690862296216021</v>
+      </c>
+      <c r="M30">
+        <v>4.7399999999999998E-2</v>
+      </c>
+      <c r="N30">
+        <v>-3.61E-2</v>
+      </c>
+      <c r="O30">
+        <v>4.3400000000000001E-2</v>
+      </c>
+      <c r="P30">
+        <v>-1.77E-2</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>